<commit_message>
New color change for xlsx file
</commit_message>
<xml_diff>
--- a/Invoice.xlsx
+++ b/Invoice.xlsx
@@ -32,7 +32,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -42,6 +42,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -63,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -74,6 +79,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -439,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="F1:T6"/>
+  <dimension ref="F1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,18 +461,19 @@
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>SHREE GANESH PRESS N COAT INDUSTRIES PRIVATE LIMITED.</t>
         </is>
       </c>
-      <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="n"/>
       <c r="Q1" s="1" t="n"/>
       <c r="R1" s="1" t="n"/>
       <c r="S1" s="1" t="n"/>
       <c r="T1" s="1" t="n"/>
+      <c r="U1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="F2" s="1" t="n"/>
@@ -476,20 +483,21 @@
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="n"/>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="2" t="inlineStr">
         <is>
           <t>27AAXPM9097J1ZI.
 Report Name: Not in GSTR 2B.
 April 23 to April 24.</t>
         </is>
       </c>
-      <c r="N2" s="1" t="n"/>
       <c r="O2" s="1" t="n"/>
       <c r="P2" s="1" t="n"/>
       <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
+      <c r="U2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="F3" s="1" t="n"/>
@@ -507,6 +515,7 @@
       <c r="R3" s="1" t="n"/>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="n"/>
+      <c r="U3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="F4" s="3" t="inlineStr">
@@ -561,25 +570,30 @@
       </c>
       <c r="P4" s="3" t="inlineStr">
         <is>
+          <t>igst_amount</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="inlineStr">
+        <is>
           <t>cgst_amount</t>
         </is>
       </c>
-      <c r="Q4" s="3" t="inlineStr">
+      <c r="R4" s="3" t="inlineStr">
         <is>
           <t>sgst_amount</t>
         </is>
       </c>
-      <c r="R4" s="3" t="inlineStr">
+      <c r="S4" s="3" t="inlineStr">
         <is>
           <t>total_tax</t>
         </is>
       </c>
-      <c r="S4" s="3" t="inlineStr">
+      <c r="T4" s="3" t="inlineStr">
         <is>
           <t>place_of_supply</t>
         </is>
       </c>
-      <c r="T4" s="3" t="inlineStr">
+      <c r="U4" s="3" t="inlineStr">
         <is>
           <t>remark</t>
         </is>
@@ -591,7 +605,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>nilesh.murkute@zencon.co.in</t>
+          <t>sachinsakh108@gmail.com</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -601,7 +615,7 @@
       </c>
       <c r="I5" s="5" t="inlineStr">
         <is>
-          <t>Nilesh Bhai</t>
+          <t>Sachin Prabhu</t>
         </is>
       </c>
       <c r="J5" s="5" t="inlineStr">
@@ -609,7 +623,7 @@
           <t>Debit Note</t>
         </is>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="6" t="n">
         <v>1639</v>
       </c>
       <c r="L5" s="4" t="n">
@@ -625,20 +639,23 @@
         <v>-6002.01</v>
       </c>
       <c r="P5" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Q5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" s="5" t="n">
+      <c r="R5" s="5" t="n">
         <v>-840.28</v>
       </c>
-      <c r="R5" s="5" t="n">
+      <c r="S5" s="5" t="n">
         <v>-1680.56</v>
       </c>
-      <c r="S5" s="5" t="inlineStr">
+      <c r="T5" s="5" t="inlineStr">
         <is>
           <t>Maharashtra</t>
         </is>
       </c>
-      <c r="T5" s="5" t="inlineStr"/>
+      <c r="U5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="F6" s="1" t="n"/>
@@ -656,6 +673,7 @@
       <c r="R6" s="1" t="n"/>
       <c r="S6" s="1" t="n"/>
       <c r="T6" s="1" t="n"/>
+      <c r="U6" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
changes for border in excel
</commit_message>
<xml_diff>
--- a/Invoice.xlsx
+++ b/Invoice.xlsx
@@ -68,17 +68,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -445,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="F1:U6"/>
+  <dimension ref="F4:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,209 +452,51 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="n"/>
-      <c r="N1" s="2" t="inlineStr">
+    <row r="4">
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="2" t="inlineStr">
         <is>
           <t>SHREE GANESH PRESS N COAT INDUSTRIES PRIVATE LIMITED.</t>
         </is>
       </c>
-      <c r="O1" s="1" t="n"/>
-      <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="n"/>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="n"/>
-      <c r="U1" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
+      <c r="T4" s="1" t="n"/>
+      <c r="U4" s="1" t="n"/>
     </row>
-    <row r="2">
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="2" t="inlineStr">
+    <row r="5">
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+      <c r="J5" s="1" t="n"/>
+      <c r="K5" s="1" t="n"/>
+      <c r="L5" s="1" t="n"/>
+      <c r="M5" s="1" t="n"/>
+      <c r="N5" s="2" t="inlineStr">
         <is>
           <t>27AAXPM9097J1ZI.
 Report Name: Not in GSTR 2B.
 April 23 to April 24.</t>
         </is>
       </c>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
-      <c r="T2" s="1" t="n"/>
-      <c r="U2" s="1" t="n"/>
-    </row>
-    <row r="3">
-      <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
-      <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="n"/>
-      <c r="K3" s="1" t="n"/>
-      <c r="L3" s="1" t="n"/>
-      <c r="M3" s="1" t="n"/>
-      <c r="N3" s="1" t="n"/>
-      <c r="O3" s="1" t="n"/>
-      <c r="P3" s="1" t="n"/>
-      <c r="Q3" s="1" t="n"/>
-      <c r="R3" s="1" t="n"/>
-      <c r="S3" s="1" t="n"/>
-      <c r="T3" s="1" t="n"/>
-      <c r="U3" s="1" t="n"/>
-    </row>
-    <row r="4">
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>gstin/uin</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>party_name</t>
-        </is>
-      </c>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>docu_type</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="inlineStr">
-        <is>
-          <t>inv_no/creditnote/debit_no</t>
-        </is>
-      </c>
-      <c r="L4" s="3" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="M4" s="3" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="N4" s="3" t="inlineStr">
-        <is>
-          <t>rate</t>
-        </is>
-      </c>
-      <c r="O4" s="3" t="inlineStr">
-        <is>
-          <t>taxable_value</t>
-        </is>
-      </c>
-      <c r="P4" s="3" t="inlineStr">
-        <is>
-          <t>igst_amount</t>
-        </is>
-      </c>
-      <c r="Q4" s="3" t="inlineStr">
-        <is>
-          <t>cgst_amount</t>
-        </is>
-      </c>
-      <c r="R4" s="3" t="inlineStr">
-        <is>
-          <t>sgst_amount</t>
-        </is>
-      </c>
-      <c r="S4" s="3" t="inlineStr">
-        <is>
-          <t>total_tax</t>
-        </is>
-      </c>
-      <c r="T4" s="3" t="inlineStr">
-        <is>
-          <t>place_of_supply</t>
-        </is>
-      </c>
-      <c r="U4" s="3" t="inlineStr">
-        <is>
-          <t>remark</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="F5" s="4" t="n">
-        <v>45323</v>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>sachinsakh108@gmail.com</t>
-        </is>
-      </c>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>27AAXPM9097J1ZI</t>
-        </is>
-      </c>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <t>Sachin Prabhu</t>
-        </is>
-      </c>
-      <c r="J5" s="5" t="inlineStr">
-        <is>
-          <t>Debit Note</t>
-        </is>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>1639</v>
-      </c>
-      <c r="L5" s="4" t="n">
-        <v>45325</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>-7682.57</v>
-      </c>
-      <c r="N5" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="O5" s="5" t="n">
-        <v>-6002.01</v>
-      </c>
-      <c r="P5" s="5" t="n">
-        <v>2500</v>
-      </c>
-      <c r="Q5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5" t="n">
-        <v>-840.28</v>
-      </c>
-      <c r="S5" s="5" t="n">
-        <v>-1680.56</v>
-      </c>
-      <c r="T5" s="5" t="inlineStr">
-        <is>
-          <t>Maharashtra</t>
-        </is>
-      </c>
-      <c r="U5" s="5" t="inlineStr"/>
+      <c r="O5" s="1" t="n"/>
+      <c r="P5" s="1" t="n"/>
+      <c r="Q5" s="1" t="n"/>
+      <c r="R5" s="1" t="n"/>
+      <c r="S5" s="1" t="n"/>
+      <c r="T5" s="1" t="n"/>
+      <c r="U5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="F6" s="1" t="n"/>
@@ -675,6 +516,146 @@
       <c r="T6" s="1" t="n"/>
       <c r="U6" s="1" t="n"/>
     </row>
+    <row r="7">
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>MONTH</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>GSTIN/UIN</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>PARTY NAME</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>DOCU TYPE</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>INV NO/CREDITNOTE/DEBIT NO</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>RATE</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>TAXABLE VALUE</t>
+        </is>
+      </c>
+      <c r="P7" s="3" t="inlineStr">
+        <is>
+          <t>IGST AMOUNT</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="inlineStr">
+        <is>
+          <t>CGST AMOUNT</t>
+        </is>
+      </c>
+      <c r="R7" s="3" t="inlineStr">
+        <is>
+          <t>SGST AMOUNT</t>
+        </is>
+      </c>
+      <c r="S7" s="3" t="inlineStr">
+        <is>
+          <t>TOTAL TAX</t>
+        </is>
+      </c>
+      <c r="T7" s="3" t="inlineStr">
+        <is>
+          <t>PLACE OF SUPPLY</t>
+        </is>
+      </c>
+      <c r="U7" s="3" t="inlineStr">
+        <is>
+          <t>REMARK</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>sachinsakh108@gmail.com</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>27AAXPM9097J1ZI</t>
+        </is>
+      </c>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t>Sachin Prabhu</t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>Debit Note</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>1639</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>45325</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>-7682.57</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>-6002.01</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>-840.28</v>
+      </c>
+      <c r="S8" s="5" t="n">
+        <v>-1680.56</v>
+      </c>
+      <c r="T8" s="1" t="inlineStr">
+        <is>
+          <t>Maharashtra</t>
+        </is>
+      </c>
+      <c r="U8" s="1" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>